<commit_message>
got most subwindows working
</commit_message>
<xml_diff>
--- a/aero.xlsx
+++ b/aero.xlsx
@@ -370,7 +370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,31 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2020-06-24</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made graphs look nicer
</commit_message>
<xml_diff>
--- a/aero.xlsx
+++ b/aero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alec/PycharmProjects/MonkeyTrackerV2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05322A5C-D9DF-C143-A88A-7BBF98D1005F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8062D490-70EC-E84F-B01A-E75521429AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -52,31 +52,10 @@
     <t>2020-07-02</t>
   </si>
   <si>
-    <t>2020-07-03</t>
-  </si>
-  <si>
-    <t>2020-07-04</t>
-  </si>
-  <si>
-    <t>2020-07-06</t>
-  </si>
-  <si>
-    <t>2020-07-07</t>
-  </si>
-  <si>
-    <t>2020-07-08</t>
-  </si>
-  <si>
-    <t>2020-07-09</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>2020-07-05</t>
   </si>
 </sst>
 </file>
@@ -479,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -511,8 +490,14 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -529,7 +514,7 @@
         <v>197</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -542,8 +527,11 @@
       <c r="C4">
         <v>12</v>
       </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -560,7 +548,7 @@
         <v>432.1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -570,125 +558,21 @@
       <c r="B6">
         <v>5</v>
       </c>
+      <c r="C6">
+        <v>10.34</v>
+      </c>
       <c r="D6">
-        <v>300</v>
+        <v>264</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
         <v>11</v>
       </c>
-      <c r="D7">
-        <v>400</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>401</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>10.9</v>
-      </c>
-      <c r="D10">
-        <v>234</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>11.4</v>
-      </c>
-      <c r="D11">
-        <v>500</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <v>10.1</v>
-      </c>
-      <c r="D12">
-        <v>123</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>287</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>